<commit_message>
Report Server: Add schedule feature
</commit_message>
<xml_diff>
--- a/rill-analysis/rill-analysis-report/src/test/resources/nu/com/rill/analysis/report/excel/Report Desinger_20120715.xlsx
+++ b/rill-analysis/rill-analysis-report/src/test/resources/nu/com/rill/analysis/report/excel/Report Desinger_20120715.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="11640"/>
+    <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="11640" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="3" r:id="rId1"/>
@@ -144,10 +144,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>地域分布</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
@@ -194,6 +190,10 @@
 {Hierarchize({[Measures].[Show Cnt], [Measures].[Ask Cnt]})} ON COLUMNS,
 {Hierarchize({{[Time].[2011]}, Filter({{[Time].[Quarter].Members}}, (Exists(Ancestor([Time].CurrentMember, [Time].[Year]), {[Time].[2011]}).Count  &gt; 0))})} ON ROWS 
 FROM [TF_CUBE]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>时间</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -594,6 +594,30 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="176" fontId="6" fillId="8" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -605,30 +629,6 @@
     </xf>
     <xf numFmtId="176" fontId="7" fillId="7" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1179,25 +1179,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="82721408"/>
-        <c:axId val="82727296"/>
+        <c:axId val="84105856"/>
+        <c:axId val="84111744"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="82721408"/>
+        <c:axId val="84105856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82727296"/>
+        <c:crossAx val="84111744"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="82727296"/>
+        <c:axId val="84111744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1205,7 +1205,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="#,##0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82721408"/>
+        <c:crossAx val="84105856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1224,7 +1224,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000122" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000122" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000133" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000133" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1316,22 +1316,22 @@
           <c:showVal val="1"/>
           <c:showCatName val="1"/>
         </c:dLbls>
-        <c:axId val="82764160"/>
-        <c:axId val="82765696"/>
+        <c:axId val="84279680"/>
+        <c:axId val="84281216"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="82764160"/>
+        <c:axId val="84279680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="82765696"/>
+        <c:crossAx val="84281216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="82765696"/>
+        <c:axId val="84281216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1357,7 +1357,7 @@
         </c:title>
         <c:numFmt formatCode="0.00_ " sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82764160"/>
+        <c:crossAx val="84279680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1373,7 +1373,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1512,24 +1512,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="89803008"/>
-        <c:axId val="89821184"/>
+        <c:axId val="84302080"/>
+        <c:axId val="84320256"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="89803008"/>
+        <c:axId val="84302080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="89821184"/>
+        <c:crossAx val="84320256"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="89821184"/>
+        <c:axId val="84320256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1537,7 +1537,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="#,##0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="89803008"/>
+        <c:crossAx val="84302080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1556,7 +1556,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1651,7 +1651,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2070,7 +2070,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="B1:AT14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E5" sqref="E5:H5"/>
     </sheetView>
   </sheetViews>
@@ -2085,99 +2085,99 @@
   <sheetData>
     <row r="1" spans="2:46" ht="5.25" customHeight="1"/>
     <row r="2" spans="2:46" ht="26.25" customHeight="1">
-      <c r="B2" s="29">
+      <c r="B2" s="21">
         <f>_input!A3</f>
         <v>2011</v>
       </c>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="30" t="s">
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
       <c r="AA2" s="14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="2:46" ht="6" customHeight="1"/>
     <row r="4" spans="2:46" ht="5.25" customHeight="1"/>
     <row r="5" spans="2:46">
-      <c r="B5" s="28" t="str">
+      <c r="B5" s="20" t="str">
         <f>_input!B2</f>
         <v>展现量</v>
       </c>
-      <c r="C5" s="28"/>
-      <c r="D5" s="28"/>
-      <c r="E5" s="31">
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="23">
         <f>_input!$B3</f>
         <v>111</v>
       </c>
-      <c r="F5" s="31"/>
-      <c r="G5" s="31"/>
-      <c r="H5" s="31"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="23"/>
     </row>
     <row r="6" spans="2:46">
-      <c r="B6" s="28" t="str">
+      <c r="B6" s="20" t="str">
         <f>_input!C2</f>
         <v>点击量</v>
       </c>
-      <c r="C6" s="28"/>
-      <c r="D6" s="28"/>
-      <c r="E6" s="31">
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="23">
         <f>_input!C3</f>
         <v>22222</v>
       </c>
-      <c r="F6" s="31"/>
-      <c r="G6" s="31"/>
-      <c r="H6" s="31"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="23"/>
     </row>
     <row r="7" spans="2:46">
-      <c r="B7" s="28" t="str">
+      <c r="B7" s="20" t="str">
         <f>_input!D2</f>
         <v>访问量</v>
       </c>
-      <c r="C7" s="28"/>
-      <c r="D7" s="28"/>
-      <c r="E7" s="31">
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="23">
         <f>_input!D3</f>
         <v>21785448</v>
       </c>
-      <c r="F7" s="31"/>
-      <c r="G7" s="31"/>
-      <c r="H7" s="31"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="23"/>
     </row>
     <row r="8" spans="2:46">
-      <c r="B8" s="28" t="str">
+      <c r="B8" s="20" t="str">
         <f>_input!E2</f>
         <v>咨询量</v>
       </c>
-      <c r="C8" s="28"/>
-      <c r="D8" s="28"/>
-      <c r="E8" s="31">
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="23">
         <f>_input!E3</f>
         <v>4793511</v>
       </c>
-      <c r="F8" s="31"/>
-      <c r="G8" s="31"/>
-      <c r="H8" s="31"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="23"/>
+      <c r="H8" s="23"/>
     </row>
     <row r="9" spans="2:46">
-      <c r="B9" s="28" t="str">
+      <c r="B9" s="20" t="str">
         <f>_input!F2</f>
         <v>订单量</v>
       </c>
-      <c r="C9" s="28"/>
-      <c r="D9" s="28"/>
-      <c r="E9" s="31">
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="23">
         <f>_input!F3</f>
         <v>134337</v>
       </c>
-      <c r="F9" s="31"/>
-      <c r="G9" s="31"/>
-      <c r="H9" s="31"/>
+      <c r="F9" s="23"/>
+      <c r="G9" s="23"/>
+      <c r="H9" s="23"/>
     </row>
     <row r="12" spans="2:46" ht="26.25" customHeight="1">
       <c r="B12" s="14" t="s">
@@ -2225,44 +2225,54 @@
       <c r="AT13" s="17"/>
     </row>
     <row r="14" spans="2:46">
-      <c r="AA14" s="20">
+      <c r="AA14" s="28">
         <f>_input!E3*1000/_input!B3</f>
         <v>43184783.783783786</v>
       </c>
-      <c r="AB14" s="21"/>
-      <c r="AC14" s="21"/>
-      <c r="AD14" s="21"/>
-      <c r="AE14" s="22">
+      <c r="AB14" s="29"/>
+      <c r="AC14" s="29"/>
+      <c r="AD14" s="29"/>
+      <c r="AE14" s="30">
         <f>_input!D22*1000/_input!C22</f>
         <v>7.3158244040475093</v>
       </c>
-      <c r="AF14" s="22"/>
-      <c r="AG14" s="22"/>
-      <c r="AH14" s="22"/>
-      <c r="AI14" s="22">
+      <c r="AF14" s="30"/>
+      <c r="AG14" s="30"/>
+      <c r="AH14" s="30"/>
+      <c r="AI14" s="30">
         <f>_input!D23*1000/_input!C23</f>
         <v>7.3528513255018675</v>
       </c>
-      <c r="AJ14" s="22"/>
-      <c r="AK14" s="22"/>
-      <c r="AL14" s="22"/>
-      <c r="AM14" s="22">
+      <c r="AJ14" s="30"/>
+      <c r="AK14" s="30"/>
+      <c r="AL14" s="30"/>
+      <c r="AM14" s="30">
         <f>_input!D24*1000/_input!C24</f>
         <v>7.3423121568627829</v>
       </c>
-      <c r="AN14" s="22"/>
-      <c r="AO14" s="22"/>
-      <c r="AP14" s="22"/>
-      <c r="AQ14" s="22">
+      <c r="AN14" s="30"/>
+      <c r="AO14" s="30"/>
+      <c r="AP14" s="30"/>
+      <c r="AQ14" s="30">
         <f>_input!D25*1000/_input!C25</f>
         <v>7.3503189475905755</v>
       </c>
-      <c r="AR14" s="22"/>
-      <c r="AS14" s="23"/>
+      <c r="AR14" s="30"/>
+      <c r="AS14" s="31"/>
       <c r="AT14" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="AA14:AD14"/>
+    <mergeCell ref="AE14:AH14"/>
+    <mergeCell ref="AI14:AL14"/>
+    <mergeCell ref="AM14:AP14"/>
+    <mergeCell ref="AQ14:AS14"/>
+    <mergeCell ref="AA13:AD13"/>
+    <mergeCell ref="AE13:AH13"/>
+    <mergeCell ref="AI13:AL13"/>
+    <mergeCell ref="AM13:AP13"/>
+    <mergeCell ref="AQ13:AS13"/>
     <mergeCell ref="B8:D8"/>
     <mergeCell ref="B9:D9"/>
     <mergeCell ref="B2:D2"/>
@@ -2275,16 +2285,6 @@
     <mergeCell ref="E7:H7"/>
     <mergeCell ref="E8:H8"/>
     <mergeCell ref="E9:H9"/>
-    <mergeCell ref="AA13:AD13"/>
-    <mergeCell ref="AE13:AH13"/>
-    <mergeCell ref="AI13:AL13"/>
-    <mergeCell ref="AM13:AP13"/>
-    <mergeCell ref="AQ13:AS13"/>
-    <mergeCell ref="AA14:AD14"/>
-    <mergeCell ref="AE14:AH14"/>
-    <mergeCell ref="AI14:AL14"/>
-    <mergeCell ref="AM14:AP14"/>
-    <mergeCell ref="AQ14:AS14"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2300,8 +2300,8 @@
   </sheetPr>
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -2318,13 +2318,13 @@
         <v>7</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D1" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="9" t="s">
         <v>19</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -2349,7 +2349,7 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B4" s="9" t="b">
         <v>1</v>
@@ -2383,7 +2383,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="18" customHeight="1" thickBot="1">
       <c r="A1" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="14.25" thickBot="1">
@@ -2428,7 +2428,7 @@
     </row>
     <row r="5" spans="1:7" ht="14.25" thickBot="1">
       <c r="A5" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="14.25" thickBot="1">
@@ -2710,7 +2710,7 @@
     </row>
     <row r="20" spans="1:7" ht="14.25" thickBot="1">
       <c r="A20" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="14.25" thickBot="1">
@@ -2779,7 +2779,7 @@
     </row>
     <row r="27" spans="1:7" ht="14.25" thickBot="1">
       <c r="A27" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="14.25" thickBot="1">
@@ -2787,7 +2787,7 @@
         <v>0</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>2</v>
@@ -2810,7 +2810,7 @@
         <v>2011</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C29" s="3">
         <v>260827852</v>
@@ -2831,7 +2831,7 @@
     <row r="30" spans="1:7" ht="14.25" thickBot="1">
       <c r="A30" s="7"/>
       <c r="B30" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C30" s="15">
         <v>392196385</v>

</xml_diff>